<commit_message>
Added excel field type checking logic
</commit_message>
<xml_diff>
--- a/public/apps/bos/excel/apps.xlsx
+++ b/public/apps/bos/excel/apps.xlsx
@@ -721,7 +721,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -741,7 +741,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -773,7 +773,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -805,7 +805,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>

</xml_diff>